<commit_message>
esa to route xlsx and route ids
</commit_message>
<xml_diff>
--- a/i9routes.xlsx
+++ b/i9routes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\demet\go\i9-backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5825954F-50A8-41D5-A4F0-A3D960866D6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2ABCD71-131B-4338-9648-D33275B0BF9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{53185A37-6B88-465F-8A8E-712CD7514683}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{53185A37-6B88-465F-8A8E-712CD7514683}"/>
   </bookViews>
   <sheets>
     <sheet name="routes" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="87">
   <si>
     <t>Functionality</t>
   </si>
@@ -276,6 +276,27 @@
   </si>
   <si>
     <t>exer id(s), favoritism val(s)</t>
+  </si>
+  <si>
+    <t>ESA</t>
+  </si>
+  <si>
+    <t>Add an exercise</t>
+  </si>
+  <si>
+    <t>Add a stretch</t>
+  </si>
+  <si>
+    <t>spec password</t>
+  </si>
+  <si>
+    <t>[]of datatype.Exercise</t>
+  </si>
+  <si>
+    <t>[]of datatype.Stretch</t>
+  </si>
+  <si>
+    <t>ID</t>
   </si>
 </sst>
 </file>
@@ -641,647 +662,783 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78B4B469-BB36-48BE-B63E-304ECB3D9CFE}">
-  <dimension ref="A1:I29"/>
+  <dimension ref="A1:J31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23" customWidth="1"/>
-    <col min="2" max="2" width="40.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19" customWidth="1"/>
-    <col min="4" max="4" width="22.5703125" customWidth="1"/>
-    <col min="5" max="5" width="20" customWidth="1"/>
-    <col min="6" max="7" width="21.42578125" customWidth="1"/>
-    <col min="8" max="8" width="12.42578125" customWidth="1"/>
-    <col min="9" max="9" width="38.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23" customWidth="1"/>
+    <col min="3" max="3" width="40.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19" customWidth="1"/>
+    <col min="5" max="5" width="22.5703125" customWidth="1"/>
+    <col min="6" max="6" width="20" customWidth="1"/>
+    <col min="7" max="8" width="21.42578125" customWidth="1"/>
+    <col min="9" max="9" width="14" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="38.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>13</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>45</v>
       </c>
-      <c r="H2" t="s">
-        <v>37</v>
-      </c>
       <c r="I2" t="s">
+        <v>37</v>
+      </c>
+      <c r="J2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
         <v>13</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>45</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>47</v>
       </c>
-      <c r="H3" t="s">
-        <v>37</v>
-      </c>
       <c r="I3" t="s">
+        <v>37</v>
+      </c>
+      <c r="J3" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
         <v>13</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>45</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>60</v>
       </c>
-      <c r="H4" t="s">
-        <v>37</v>
-      </c>
       <c r="I4" t="s">
+        <v>37</v>
+      </c>
+      <c r="J4" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
         <v>13</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>45</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>61</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>72</v>
       </c>
-      <c r="H5" t="s">
-        <v>37</v>
-      </c>
       <c r="I5" t="s">
+        <v>37</v>
+      </c>
+      <c r="J5" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
         <v>13</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>45</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>62</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>72</v>
       </c>
-      <c r="H6" t="s">
-        <v>37</v>
-      </c>
       <c r="I6" t="s">
+        <v>37</v>
+      </c>
+      <c r="J6" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
         <v>13</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>45</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>63</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>72</v>
       </c>
-      <c r="H7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="I7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
         <v>13</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>45</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>66</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>72</v>
       </c>
-      <c r="H8" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="I8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
         <v>42</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>46</v>
       </c>
-      <c r="H9" t="s">
-        <v>37</v>
-      </c>
       <c r="I9" t="s">
+        <v>37</v>
+      </c>
+      <c r="J9" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
         <v>42</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>56</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>46</v>
       </c>
-      <c r="H10" t="s">
-        <v>37</v>
-      </c>
       <c r="I10" t="s">
+        <v>37</v>
+      </c>
+      <c r="J10" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
         <v>42</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>43</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>46</v>
       </c>
-      <c r="H11" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="I11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
         <v>42</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>59</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="D12" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>46</v>
       </c>
-      <c r="H12" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="I12" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
         <v>21</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="D13" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>45</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
         <v>72</v>
       </c>
-      <c r="H13" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="I13" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
         <v>21</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>65</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="D14" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>45</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>68</v>
       </c>
-      <c r="F14" t="s">
+      <c r="G14" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="I14" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
         <v>21</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="D15" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>45</v>
       </c>
-      <c r="G15" t="s">
+      <c r="H15" t="s">
         <v>73</v>
       </c>
-      <c r="H15" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="I15" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
         <v>21</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="D16" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>48</v>
       </c>
-      <c r="F16" t="s">
+      <c r="G16" t="s">
         <v>74</v>
       </c>
-      <c r="H16" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="I16" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
         <v>21</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="D17" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>49</v>
       </c>
-      <c r="F17" t="s">
+      <c r="G17" t="s">
         <v>75</v>
       </c>
-      <c r="H17" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="I17" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
         <v>21</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="D18" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>48</v>
       </c>
-      <c r="H18" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="I18" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
         <v>21</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>18</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="D19" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>49</v>
       </c>
-      <c r="G19" t="s">
+      <c r="H19" t="s">
         <v>76</v>
       </c>
-      <c r="H19" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="I19" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
         <v>31</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>22</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="D20" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>46</v>
       </c>
-      <c r="E20" t="s">
+      <c r="F20" t="s">
         <v>67</v>
       </c>
-      <c r="H20" t="s">
-        <v>37</v>
-      </c>
       <c r="I20" t="s">
+        <v>37</v>
+      </c>
+      <c r="J20" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
         <v>29</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
         <v>23</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="D21" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>46</v>
       </c>
-      <c r="E21" t="s">
+      <c r="F21" t="s">
         <v>70</v>
       </c>
-      <c r="H21" t="s">
-        <v>37</v>
-      </c>
       <c r="I21" t="s">
+        <v>37</v>
+      </c>
+      <c r="J21" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
         <v>29</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
         <v>24</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="D22" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D22" t="s">
+      <c r="E22" t="s">
         <v>46</v>
       </c>
-      <c r="E22" t="s">
+      <c r="F22" t="s">
         <v>71</v>
       </c>
-      <c r="H22" t="s">
-        <v>37</v>
-      </c>
       <c r="I22" t="s">
+        <v>37</v>
+      </c>
+      <c r="J22" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
         <v>29</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
         <v>25</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="D23" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D23" t="s">
+      <c r="E23" t="s">
         <v>46</v>
       </c>
-      <c r="E23" t="s">
+      <c r="F23" t="s">
         <v>69</v>
       </c>
-      <c r="H23" t="s">
-        <v>37</v>
-      </c>
       <c r="I23" t="s">
+        <v>37</v>
+      </c>
+      <c r="J23" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
         <v>30</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" t="s">
         <v>26</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="D24" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D24" t="s">
+      <c r="E24" t="s">
         <v>46</v>
       </c>
-      <c r="E24" t="s">
+      <c r="F24" t="s">
         <v>70</v>
       </c>
-      <c r="H24" t="s">
-        <v>37</v>
-      </c>
       <c r="I24" t="s">
+        <v>37</v>
+      </c>
+      <c r="J24" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
         <v>30</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C25" t="s">
         <v>27</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="D25" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D25" t="s">
+      <c r="E25" t="s">
         <v>46</v>
       </c>
-      <c r="E25" t="s">
+      <c r="F25" t="s">
         <v>71</v>
       </c>
-      <c r="H25" t="s">
-        <v>37</v>
-      </c>
       <c r="I25" t="s">
+        <v>37</v>
+      </c>
+      <c r="J25" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
         <v>30</v>
       </c>
-      <c r="B26" t="s">
+      <c r="C26" t="s">
         <v>28</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="D26" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D26" t="s">
+      <c r="E26" t="s">
         <v>46</v>
       </c>
-      <c r="E26" t="s">
+      <c r="F26" t="s">
         <v>69</v>
       </c>
-      <c r="H26" t="s">
-        <v>37</v>
-      </c>
       <c r="I26" t="s">
+        <v>37</v>
+      </c>
+      <c r="J26" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
         <v>33</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C27" t="s">
         <v>34</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="D27" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D27" t="s">
+      <c r="E27" t="s">
         <v>46</v>
       </c>
-      <c r="E27" t="s">
+      <c r="F27" t="s">
         <v>70</v>
       </c>
-      <c r="H27" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="I27" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
         <v>33</v>
       </c>
-      <c r="B28" t="s">
+      <c r="C28" t="s">
         <v>35</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="D28" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D28" t="s">
+      <c r="E28" t="s">
         <v>46</v>
       </c>
-      <c r="E28" t="s">
+      <c r="F28" t="s">
         <v>71</v>
       </c>
-      <c r="H28" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="I28" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
         <v>33</v>
       </c>
-      <c r="B29" t="s">
+      <c r="C29" t="s">
         <v>36</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="D29" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D29" t="s">
+      <c r="E29" t="s">
         <v>46</v>
       </c>
-      <c r="E29" t="s">
+      <c r="F29" t="s">
         <v>69</v>
       </c>
-      <c r="H29" t="s">
-        <v>37</v>
+      <c r="I29" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>80</v>
+      </c>
+      <c r="C30" t="s">
+        <v>81</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E30" t="s">
+        <v>49</v>
+      </c>
+      <c r="I30" t="s">
+        <v>83</v>
+      </c>
+      <c r="J30" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>80</v>
+      </c>
+      <c r="C31" t="s">
+        <v>82</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E31" t="s">
+        <v>48</v>
+      </c>
+      <c r="I31" t="s">
+        <v>83</v>
+      </c>
+      <c r="J31" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
naming plus fixes for wo views
</commit_message>
<xml_diff>
--- a/i9routes.xlsx
+++ b/i9routes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jam/go/i9-backend/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5193CCD9-BC51-9D48-A823-3BD6FE61F050}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{793DC4E1-7B91-774B-BEE6-1F1642A396AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="17280" yWindow="760" windowWidth="17280" windowHeight="20260" xr2:uid="{53185A37-6B88-465F-8A8E-712CD7514683}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="95">
   <si>
     <t>Functionality</t>
   </si>
@@ -312,6 +312,15 @@
   </si>
   <si>
     <t>PATCH</t>
+  </si>
+  <si>
+    <t>View one stretch workout for a user</t>
+  </si>
+  <si>
+    <t>View stretch workouts for a user</t>
+  </si>
+  <si>
+    <t>/workouts/stretch</t>
   </si>
 </sst>
 </file>
@@ -684,10 +693,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78B4B469-BB36-48BE-B63E-304ECB3D9CFE}">
-  <dimension ref="A1:L32"/>
+  <dimension ref="A1:L34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -804,7 +813,7 @@
     <row r="4" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4"/>
       <c r="B4" s="3">
-        <f t="shared" ref="B4:B32" si="0">B3+1</f>
+        <f t="shared" ref="B4:B34" si="0">B3+1</f>
         <v>3</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -1182,63 +1191,59 @@
       </c>
     </row>
     <row r="16" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A16" t="b">
-        <v>1</v>
-      </c>
+      <c r="A16"/>
       <c r="B16" s="3">
-        <f t="shared" si="0"/>
+        <f>B15+1</f>
         <v>15</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>19</v>
+        <v>92</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>40</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>47</v>
+        <v>94</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J16" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="L16" s="2" t="s">
-        <v>80</v>
+      <c r="K16" s="2" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="17" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A17" t="b">
-        <v>1</v>
-      </c>
+      <c r="A17"/>
       <c r="B17" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="B17:B34" si="1">B16+1</f>
         <v>16</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>20</v>
+        <v>93</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>40</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>64</v>
+        <v>94</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>89</v>
       </c>
       <c r="J17" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="L17" s="2" t="s">
-        <v>80</v>
+      <c r="K17" s="2" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="18" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -1246,14 +1251,14 @@
         <v>1</v>
       </c>
       <c r="B18" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>17</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>40</v>
@@ -1261,8 +1266,8 @@
       <c r="F18" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="I18" s="2" t="s">
-        <v>65</v>
+      <c r="H18" s="2" t="s">
+        <v>63</v>
       </c>
       <c r="J18" s="2" t="s">
         <v>37</v>
@@ -1276,14 +1281,14 @@
         <v>1</v>
       </c>
       <c r="B19" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>18</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>40</v>
@@ -1291,8 +1296,8 @@
       <c r="F19" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="I19" s="2" t="s">
-        <v>65</v>
+      <c r="H19" s="2" t="s">
+        <v>64</v>
       </c>
       <c r="J19" s="2" t="s">
         <v>37</v>
@@ -1306,29 +1311,26 @@
         <v>1</v>
       </c>
       <c r="B20" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>57</v>
+        <v>47</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>65</v>
       </c>
       <c r="J20" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="K20" s="2" t="s">
-        <v>74</v>
       </c>
       <c r="L20" s="2" t="s">
         <v>80</v>
@@ -1339,29 +1341,26 @@
         <v>1</v>
       </c>
       <c r="B21" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>60</v>
+        <v>48</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>65</v>
       </c>
       <c r="J21" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="K21" s="2" t="s">
-        <v>75</v>
       </c>
       <c r="L21" s="2" t="s">
         <v>80</v>
@@ -1372,14 +1371,14 @@
         <v>1</v>
       </c>
       <c r="B22" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>21</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>39</v>
@@ -1388,13 +1387,13 @@
         <v>45</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="J22" s="2" t="s">
         <v>37</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="L22" s="2" t="s">
         <v>80</v>
@@ -1405,14 +1404,14 @@
         <v>1</v>
       </c>
       <c r="B23" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>22</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>29</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>39</v>
@@ -1421,13 +1420,13 @@
         <v>45</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="J23" s="2" t="s">
         <v>37</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="L23" s="2" t="s">
         <v>80</v>
@@ -1438,14 +1437,14 @@
         <v>1</v>
       </c>
       <c r="B24" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>23</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>29</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>82</v>
+        <v>24</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>39</v>
@@ -1454,13 +1453,13 @@
         <v>45</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>83</v>
+        <v>61</v>
       </c>
       <c r="J24" s="2" t="s">
         <v>37</v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="L24" s="2" t="s">
         <v>80</v>
@@ -1471,29 +1470,29 @@
         <v>1</v>
       </c>
       <c r="B25" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>24</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F25" s="2" t="s">
         <v>45</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J25" s="2" t="s">
         <v>37</v>
       </c>
       <c r="K25" s="2" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="L25" s="2" t="s">
         <v>80</v>
@@ -1504,29 +1503,29 @@
         <v>1</v>
       </c>
       <c r="B26" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>25</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>27</v>
+        <v>82</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F26" s="2" t="s">
         <v>45</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>61</v>
+        <v>83</v>
       </c>
       <c r="J26" s="2" t="s">
         <v>37</v>
       </c>
       <c r="K26" s="2" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="L26" s="2" t="s">
         <v>80</v>
@@ -1537,14 +1536,14 @@
         <v>1</v>
       </c>
       <c r="B27" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>26</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>30</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>41</v>
@@ -1553,7 +1552,7 @@
         <v>45</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="J27" s="2" t="s">
         <v>37</v>
@@ -1570,14 +1569,14 @@
         <v>1</v>
       </c>
       <c r="B28" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>27</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>30</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>84</v>
+        <v>27</v>
       </c>
       <c r="E28" s="3" t="s">
         <v>41</v>
@@ -1586,13 +1585,13 @@
         <v>45</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>83</v>
+        <v>61</v>
       </c>
       <c r="J28" s="2" t="s">
         <v>37</v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="L28" s="2" t="s">
         <v>80</v>
@@ -1603,14 +1602,14 @@
         <v>1</v>
       </c>
       <c r="B29" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>28</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="E29" s="3" t="s">
         <v>41</v>
@@ -1619,13 +1618,13 @@
         <v>45</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J29" s="2" t="s">
         <v>37</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="L29" s="2" t="s">
         <v>80</v>
@@ -1636,14 +1635,14 @@
         <v>1</v>
       </c>
       <c r="B30" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>29</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>35</v>
+        <v>84</v>
       </c>
       <c r="E30" s="3" t="s">
         <v>41</v>
@@ -1652,13 +1651,13 @@
         <v>45</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>61</v>
+        <v>83</v>
       </c>
       <c r="J30" s="2" t="s">
         <v>37</v>
       </c>
       <c r="K30" s="2" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="L30" s="2" t="s">
         <v>80</v>
@@ -1669,14 +1668,14 @@
         <v>1</v>
       </c>
       <c r="B31" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>33</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E31" s="3" t="s">
         <v>41</v>
@@ -1685,7 +1684,7 @@
         <v>45</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="J31" s="2" t="s">
         <v>37</v>
@@ -1702,14 +1701,14 @@
         <v>1</v>
       </c>
       <c r="B32" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>31</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>33</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>85</v>
+        <v>35</v>
       </c>
       <c r="E32" s="3" t="s">
         <v>41</v>
@@ -1718,7 +1717,7 @@
         <v>45</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>83</v>
+        <v>61</v>
       </c>
       <c r="J32" s="2" t="s">
         <v>37</v>
@@ -1727,6 +1726,72 @@
         <v>72</v>
       </c>
       <c r="L32" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A33" t="b">
+        <v>1</v>
+      </c>
+      <c r="B33" s="3">
+        <f t="shared" si="1"/>
+        <v>32</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="J33" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="K33" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="L33" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A34" t="b">
+        <v>1</v>
+      </c>
+      <c r="B34" s="3">
+        <f t="shared" si="1"/>
+        <v>33</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="J34" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="K34" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="L34" s="2" t="s">
         <v>80</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixes and adds for adapt wo
</commit_message>
<xml_diff>
--- a/i9routes.xlsx
+++ b/i9routes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jam/go/i9-backend/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{793DC4E1-7B91-774B-BEE6-1F1642A396AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE364852-C67B-BA42-9579-EC3D937FE263}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="17280" yWindow="760" windowWidth="17280" windowHeight="20260" xr2:uid="{53185A37-6B88-465F-8A8E-712CD7514683}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="96">
   <si>
     <t>Functionality</t>
   </si>
@@ -321,6 +321,9 @@
   </si>
   <si>
     <t>/workouts/stretch</t>
+  </si>
+  <si>
+    <t>difficulty, as new, [until JWT] userID</t>
   </si>
 </sst>
 </file>
@@ -695,8 +698,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78B4B469-BB36-48BE-B63E-304ECB3D9CFE}">
   <dimension ref="A1:L34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -753,7 +756,9 @@
       </c>
     </row>
     <row r="2" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2"/>
+      <c r="A2" t="b">
+        <v>1</v>
+      </c>
       <c r="B2" s="3">
         <v>1</v>
       </c>
@@ -780,7 +785,9 @@
       </c>
     </row>
     <row r="3" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3"/>
+      <c r="A3" t="b">
+        <v>1</v>
+      </c>
       <c r="B3" s="3">
         <f>B2+1</f>
         <v>2</v>
@@ -811,7 +818,9 @@
       </c>
     </row>
     <row r="4" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4"/>
+      <c r="A4" t="b">
+        <v>1</v>
+      </c>
       <c r="B4" s="3">
         <f t="shared" ref="B4:B34" si="0">B3+1</f>
         <v>3</v>
@@ -842,7 +851,9 @@
       </c>
     </row>
     <row r="5" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5"/>
+      <c r="A5" t="b">
+        <v>1</v>
+      </c>
       <c r="B5" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -876,7 +887,9 @@
       </c>
     </row>
     <row r="6" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6"/>
+      <c r="A6" t="b">
+        <v>1</v>
+      </c>
       <c r="B6" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -934,7 +947,7 @@
         <v>37</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="L7" s="2" t="s">
         <v>80</v>
@@ -1095,7 +1108,9 @@
       </c>
     </row>
     <row r="13" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13"/>
+      <c r="A13" t="b">
+        <v>1</v>
+      </c>
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1126,7 +1141,9 @@
       </c>
     </row>
     <row r="14" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14"/>
+      <c r="A14" t="b">
+        <v>1</v>
+      </c>
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1160,7 +1177,9 @@
       </c>
     </row>
     <row r="15" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15"/>
+      <c r="A15" t="b">
+        <v>1</v>
+      </c>
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1191,7 +1210,9 @@
       </c>
     </row>
     <row r="16" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A16"/>
+      <c r="A16" t="b">
+        <v>1</v>
+      </c>
       <c r="B16" s="3">
         <f>B15+1</f>
         <v>15</v>
@@ -1219,7 +1240,9 @@
       </c>
     </row>
     <row r="17" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A17"/>
+      <c r="A17" t="b">
+        <v>1</v>
+      </c>
       <c r="B17" s="3">
         <f t="shared" ref="B17:B34" si="1">B16+1</f>
         <v>16</v>

</xml_diff>

<commit_message>
start transition to api auth
</commit_message>
<xml_diff>
--- a/i9routes.xlsx
+++ b/i9routes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jam/go/i9-backend/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE364852-C67B-BA42-9579-EC3D937FE263}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2CFD551-7399-824B-8C99-3E708E41C773}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="17280" yWindow="760" windowWidth="17280" windowHeight="20260" xr2:uid="{53185A37-6B88-465F-8A8E-712CD7514683}"/>
   </bookViews>
@@ -698,8 +698,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78B4B469-BB36-48BE-B63E-304ECB3D9CFE}">
   <dimension ref="A1:L34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -920,7 +920,9 @@
       </c>
     </row>
     <row r="7" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7"/>
+      <c r="A7" t="b">
+        <v>1</v>
+      </c>
       <c r="B7" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -954,7 +956,9 @@
       </c>
     </row>
     <row r="8" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8"/>
+      <c r="A8" t="b">
+        <v>1</v>
+      </c>
       <c r="B8" s="3">
         <f t="shared" si="0"/>
         <v>7</v>

</xml_diff>

<commit_message>
merge local and auth user
</commit_message>
<xml_diff>
--- a/i9routes.xlsx
+++ b/i9routes.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jam/go/i9-backend/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACAA79BF-3105-484F-BFB2-C8C5FFE88CDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16DF9FD3-970F-AF49-84EA-C078DD3E9681}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20500" xr2:uid="{53185A37-6B88-465F-8A8E-712CD7514683}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="97">
   <si>
     <t>Functionality</t>
   </si>
@@ -278,9 +278,6 @@
     <t xml:space="preserve">time, </t>
   </si>
   <si>
-    <t xml:space="preserve">[later] time, </t>
-  </si>
-  <si>
     <t xml:space="preserve">ratings array, </t>
   </si>
   <si>
@@ -318,6 +315,18 @@
   </si>
   <si>
     <t>name,</t>
+  </si>
+  <si>
+    <t>Merge local user to new user</t>
+  </si>
+  <si>
+    <t>PA</t>
+  </si>
+  <si>
+    <t>/merge</t>
+  </si>
+  <si>
+    <t>old JWT,</t>
   </si>
 </sst>
 </file>
@@ -690,10 +699,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78B4B469-BB36-48BE-B63E-304ECB3D9CFE}">
-  <dimension ref="A1:K35"/>
+  <dimension ref="A1:K36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -806,7 +815,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="3">
-        <f t="shared" ref="B4:B35" si="0">B3+1</f>
+        <f t="shared" ref="B4:B36" si="0">B3+1</f>
         <v>3</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -828,7 +837,7 @@
         <v>37</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -861,7 +870,7 @@
         <v>37</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -891,7 +900,7 @@
         <v>37</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="7" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -924,7 +933,7 @@
         <v>37</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -957,7 +966,7 @@
         <v>37</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="9" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -972,7 +981,7 @@
         <v>42</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>39</v>
@@ -981,13 +990,13 @@
         <v>45</v>
       </c>
       <c r="G9" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="K9" s="2" t="s">
         <v>92</v>
-      </c>
-      <c r="J9" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="K9" s="2" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="10" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -1014,7 +1023,7 @@
         <v>37</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="11" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -1041,7 +1050,7 @@
         <v>37</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="12" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -1056,16 +1065,22 @@
         <v>42</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>43</v>
+        <v>93</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>41</v>
+        <v>94</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>45</v>
       </c>
+      <c r="G12" s="2" t="s">
+        <v>95</v>
+      </c>
       <c r="J12" s="2" t="s">
         <v>37</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="13" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -1080,10 +1095,10 @@
         <v>42</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>45</v>
@@ -1101,19 +1116,16 @@
         <v>13</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>21</v>
+        <v>42</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>14</v>
+        <v>50</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>40</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
       <c r="J14" s="2" t="s">
         <v>37</v>
@@ -1131,7 +1143,7 @@
         <v>21</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>56</v>
+        <v>14</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>40</v>
@@ -1139,9 +1151,6 @@
       <c r="F15" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="G15" s="2" t="s">
-        <v>58</v>
-      </c>
       <c r="H15" s="2" t="s">
         <v>62</v>
       </c>
@@ -1161,7 +1170,7 @@
         <v>21</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>15</v>
+        <v>56</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>40</v>
@@ -1169,8 +1178,11 @@
       <c r="F16" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="I16" s="2" t="s">
-        <v>72</v>
+      <c r="G16" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>62</v>
       </c>
       <c r="J16" s="2" t="s">
         <v>37</v>
@@ -1188,16 +1200,16 @@
         <v>21</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>75</v>
+        <v>15</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>40</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>62</v>
+        <v>44</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>72</v>
       </c>
       <c r="J17" s="2" t="s">
         <v>37</v>
@@ -1215,7 +1227,7 @@
         <v>21</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>40</v>
@@ -1223,8 +1235,8 @@
       <c r="F18" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="I18" s="2" t="s">
-        <v>72</v>
+      <c r="H18" s="2" t="s">
+        <v>62</v>
       </c>
       <c r="J18" s="2" t="s">
         <v>37</v>
@@ -1242,16 +1254,16 @@
         <v>21</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>19</v>
+        <v>76</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>40</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="H19" s="2" t="s">
-        <v>63</v>
+        <v>77</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>72</v>
       </c>
       <c r="J19" s="2" t="s">
         <v>37</v>
@@ -1269,16 +1281,16 @@
         <v>21</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>40</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J20" s="2" t="s">
         <v>37</v>
@@ -1296,16 +1308,16 @@
         <v>21</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>40</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="I21" s="2" t="s">
-        <v>65</v>
+        <v>48</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>64</v>
       </c>
       <c r="J21" s="2" t="s">
         <v>37</v>
@@ -1323,13 +1335,13 @@
         <v>21</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>40</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I22" s="2" t="s">
         <v>65</v>
@@ -1347,25 +1359,22 @@
         <v>22</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>57</v>
+        <v>48</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>65</v>
       </c>
       <c r="J23" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="K23" s="2" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="24" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -1377,10 +1386,10 @@
         <v>23</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>39</v>
@@ -1389,13 +1398,13 @@
         <v>45</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="J24" s="2" t="s">
         <v>37</v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="25" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -1410,7 +1419,7 @@
         <v>29</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E25" s="3" t="s">
         <v>39</v>
@@ -1419,13 +1428,13 @@
         <v>45</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J25" s="2" t="s">
         <v>37</v>
       </c>
       <c r="K25" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="26" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -1440,7 +1449,7 @@
         <v>29</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>39</v>
@@ -1449,13 +1458,13 @@
         <v>45</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="J26" s="2" t="s">
         <v>37</v>
       </c>
       <c r="K26" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="27" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -1470,7 +1479,7 @@
         <v>29</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>67</v>
+        <v>25</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>39</v>
@@ -1479,13 +1488,13 @@
         <v>45</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="J27" s="2" t="s">
         <v>37</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="28" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -1497,25 +1506,25 @@
         <v>27</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>26</v>
+        <v>67</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F28" s="2" t="s">
         <v>45</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="J28" s="2" t="s">
         <v>37</v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="29" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -1530,7 +1539,7 @@
         <v>30</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E29" s="3" t="s">
         <v>41</v>
@@ -1539,13 +1548,13 @@
         <v>45</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J29" s="2" t="s">
         <v>37</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="30" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -1560,7 +1569,7 @@
         <v>30</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E30" s="3" t="s">
         <v>41</v>
@@ -1569,7 +1578,7 @@
         <v>45</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="J30" s="2" t="s">
         <v>37</v>
@@ -1590,7 +1599,7 @@
         <v>30</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>69</v>
+        <v>28</v>
       </c>
       <c r="E31" s="3" t="s">
         <v>41</v>
@@ -1599,13 +1608,13 @@
         <v>45</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="J31" s="2" t="s">
         <v>37</v>
       </c>
       <c r="K31" s="2" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="32" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -1617,10 +1626,10 @@
         <v>31</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>34</v>
+        <v>69</v>
       </c>
       <c r="E32" s="3" t="s">
         <v>41</v>
@@ -1629,10 +1638,13 @@
         <v>45</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="J32" s="2" t="s">
         <v>37</v>
+      </c>
+      <c r="K32" s="2" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="33" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -1647,7 +1659,7 @@
         <v>33</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E33" s="3" t="s">
         <v>41</v>
@@ -1656,7 +1668,7 @@
         <v>45</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J33" s="2" t="s">
         <v>37</v>
@@ -1674,7 +1686,7 @@
         <v>33</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E34" s="3" t="s">
         <v>41</v>
@@ -1683,7 +1695,7 @@
         <v>45</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="J34" s="2" t="s">
         <v>37</v>
@@ -1701,7 +1713,7 @@
         <v>33</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>70</v>
+        <v>36</v>
       </c>
       <c r="E35" s="3" t="s">
         <v>41</v>
@@ -1710,9 +1722,36 @@
         <v>45</v>
       </c>
       <c r="G35" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="J35" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A36" t="b">
+        <v>1</v>
+      </c>
+      <c r="B36" s="3">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G36" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="J35" s="2" t="s">
+      <c r="J36" s="2" t="s">
         <v>37</v>
       </c>
     </row>

</xml_diff>